<commit_message>
Add example for Excel Import
</commit_message>
<xml_diff>
--- a/AutoScout24_1_0/TestData/TestData_Cars.xlsx
+++ b/AutoScout24_1_0/TestData/TestData_Cars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\TRIO.TestAutomation\Demos\AutoScout24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\TRIO.TestAutomation\Demos\AutoScout24\AutoScout24_1_0\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC435430-2DCD-4E69-8509-A3AEE1A39B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8239043F-F671-454A-8F81-D36E1CC6F58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23325" yWindow="2850" windowWidth="21600" windowHeight="11295" xr2:uid="{16D008AA-0258-4684-B8AD-F3A177CAFC88}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16D008AA-0258-4684-B8AD-F3A177CAFC88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Automatic</t>
   </si>
   <si>
-    <t>Alfa Romea</t>
-  </si>
-  <si>
     <t>Giulia</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Second hand</t>
+  </si>
+  <si>
+    <t>Alfa Romeo</t>
   </si>
 </sst>
 </file>
@@ -103,7 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -144,7 +144,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -464,7 +464,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +499,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -533,10 +533,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>48890</v>
@@ -548,10 +548,10 @@
         <v>7648</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>280</v>
@@ -562,10 +562,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="1">
         <v>35000</v>
@@ -580,7 +580,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4">
         <v>306</v>

</xml_diff>